<commit_message>
feat: [PBL6] Range F0 from 60 to 400 Hz for cepstral method
</commit_message>
<xml_diff>
--- a/speech_processing/analysis/results/cepstrum/F0_comparison_FHU_RE_005.xlsx
+++ b/speech_processing/analysis/results/cepstrum/F0_comparison_FHU_RE_005.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D207"/>
+  <dimension ref="A1:D195"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -466,7 +466,7 @@
         <v>181.3748321533203</v>
       </c>
       <c r="D2" t="n">
-        <v>30.3664521389563</v>
+        <v>26.93401682116321</v>
       </c>
     </row>
     <row r="3">
@@ -496,10 +496,10 @@
         <v>196.0837554931641</v>
       </c>
       <c r="B5" t="n">
-        <v>386.84</v>
+        <v>393.75</v>
       </c>
       <c r="C5" t="n">
-        <v>190.7562445068359</v>
+        <v>197.6662445068359</v>
       </c>
     </row>
     <row r="6">
@@ -507,10 +507,10 @@
         <v>181.6147308349609</v>
       </c>
       <c r="B6" t="n">
-        <v>386.84</v>
+        <v>393.75</v>
       </c>
       <c r="C6" t="n">
-        <v>205.225269165039</v>
+        <v>212.1352691650391</v>
       </c>
     </row>
     <row r="7">
@@ -573,10 +573,10 @@
         <v>198.1161651611328</v>
       </c>
       <c r="B12" t="n">
-        <v>216.18</v>
+        <v>196.88</v>
       </c>
       <c r="C12" t="n">
-        <v>18.06383483886719</v>
+        <v>1.236165161132817</v>
       </c>
     </row>
     <row r="13">
@@ -595,10 +595,10 @@
         <v>214.4307861328125</v>
       </c>
       <c r="B14" t="n">
-        <v>196.88</v>
+        <v>216.18</v>
       </c>
       <c r="C14" t="n">
-        <v>17.5507861328125</v>
+        <v>1.749213867187507</v>
       </c>
     </row>
     <row r="15">
@@ -606,10 +606,10 @@
         <v>263.6256408691406</v>
       </c>
       <c r="B15" t="n">
-        <v>245</v>
+        <v>272.22</v>
       </c>
       <c r="C15" t="n">
-        <v>18.62564086914062</v>
+        <v>8.594359130859402</v>
       </c>
     </row>
     <row r="16">
@@ -617,10 +617,10 @@
         <v>259.2406005859375</v>
       </c>
       <c r="B16" t="n">
-        <v>245</v>
+        <v>256.4</v>
       </c>
       <c r="C16" t="n">
-        <v>14.2406005859375</v>
+        <v>2.840600585937523</v>
       </c>
     </row>
     <row r="17">
@@ -672,10 +672,10 @@
         <v>200.0549163818359</v>
       </c>
       <c r="B21" t="n">
-        <v>206.07</v>
+        <v>204.17</v>
       </c>
       <c r="C21" t="n">
-        <v>6.015083618164056</v>
+        <v>4.11508361816405</v>
       </c>
     </row>
     <row r="22">
@@ -694,10 +694,10 @@
         <v>187.0814361572266</v>
       </c>
       <c r="B23" t="n">
-        <v>190.09</v>
+        <v>188.46</v>
       </c>
       <c r="C23" t="n">
-        <v>3.008563842773441</v>
+        <v>1.378563842773445</v>
       </c>
     </row>
     <row r="24">
@@ -705,10 +705,10 @@
         <v>188.0236663818359</v>
       </c>
       <c r="B24" t="n">
-        <v>190.09</v>
+        <v>186.86</v>
       </c>
       <c r="C24" t="n">
-        <v>2.066333618164066</v>
+        <v>1.163666381835924</v>
       </c>
     </row>
     <row r="25">
@@ -727,10 +727,10 @@
         <v>199.7234191894531</v>
       </c>
       <c r="B26" t="n">
-        <v>190.09</v>
+        <v>195.13</v>
       </c>
       <c r="C26" t="n">
-        <v>9.633419189453122</v>
+        <v>4.59341918945313</v>
       </c>
     </row>
     <row r="27">
@@ -738,164 +738,164 @@
         <v>211.3448181152344</v>
       </c>
       <c r="B27" t="n">
-        <v>195.13</v>
+        <v>204.17</v>
       </c>
       <c r="C27" t="n">
-        <v>16.21481811523438</v>
+        <v>7.174818115234388</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="n">
-        <v>229.1416320800781</v>
+        <v>250.4183349609375</v>
       </c>
       <c r="B28" t="n">
-        <v>195.13</v>
+        <v>239.67</v>
       </c>
       <c r="C28" t="n">
-        <v>34.01163208007813</v>
+        <v>10.74833496093751</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="n">
-        <v>250.4183349609375</v>
+        <v>328.3784790039062</v>
       </c>
       <c r="B29" t="n">
-        <v>204.17</v>
+        <v>319.57</v>
       </c>
       <c r="C29" t="n">
-        <v>46.24833496093751</v>
+        <v>8.808479003906257</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="n">
-        <v>282.8031005859375</v>
+        <v>364.5834655761719</v>
       </c>
       <c r="B30" t="n">
-        <v>239.67</v>
+        <v>350</v>
       </c>
       <c r="C30" t="n">
-        <v>43.13310058593751</v>
+        <v>14.58346557617188</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="n">
-        <v>328.3784790039062</v>
+        <v>190.9148712158203</v>
       </c>
       <c r="B31" t="n">
-        <v>319.57</v>
+        <v>373.73</v>
       </c>
       <c r="C31" t="n">
-        <v>8.808479003906257</v>
+        <v>182.8151287841797</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="n">
-        <v>364.5834655761719</v>
+        <v>194.8218841552734</v>
       </c>
       <c r="B32" t="n">
-        <v>350</v>
+        <v>393.75</v>
       </c>
       <c r="C32" t="n">
-        <v>14.58346557617188</v>
+        <v>198.9281158447266</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="n">
-        <v>190.9148712158203</v>
+        <v>253.9782104492188</v>
       </c>
       <c r="B33" t="n">
-        <v>350</v>
+        <v>253.45</v>
       </c>
       <c r="C33" t="n">
-        <v>159.0851287841797</v>
+        <v>0.5282104492187614</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="n">
-        <v>194.8218841552734</v>
+        <v>254.3526611328125</v>
       </c>
       <c r="B34" t="n">
-        <v>350</v>
+        <v>253.45</v>
       </c>
       <c r="C34" t="n">
-        <v>155.1781158447266</v>
+        <v>0.9026611328125114</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="n">
-        <v>254.3526611328125</v>
+        <v>301.6283874511719</v>
       </c>
       <c r="B35" t="n">
-        <v>253.45</v>
+        <v>302.05</v>
       </c>
       <c r="C35" t="n">
-        <v>0.9026611328125114</v>
+        <v>0.4216125488281364</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="n">
-        <v>301.6137390136719</v>
+        <v>298.5026550292969</v>
       </c>
       <c r="B36" t="n">
-        <v>253.45</v>
+        <v>302.05</v>
       </c>
       <c r="C36" t="n">
-        <v>48.16373901367189</v>
+        <v>3.547344970703136</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="n">
-        <v>301.6283874511719</v>
+        <v>290.8064575195312</v>
       </c>
       <c r="B37" t="n">
         <v>294</v>
       </c>
       <c r="C37" t="n">
-        <v>7.628387451171875</v>
+        <v>3.19354248046875</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="n">
-        <v>298.5026550292969</v>
+        <v>255.4906463623047</v>
       </c>
       <c r="B38" t="n">
-        <v>294</v>
+        <v>272.22</v>
       </c>
       <c r="C38" t="n">
-        <v>4.502655029296875</v>
+        <v>16.72935363769534</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="n">
-        <v>290.8064575195312</v>
+        <v>228.4983978271484</v>
       </c>
       <c r="B39" t="n">
-        <v>294</v>
+        <v>242.31</v>
       </c>
       <c r="C39" t="n">
-        <v>3.19354248046875</v>
+        <v>13.81160217285156</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="n">
-        <v>255.4906463623047</v>
+        <v>0</v>
       </c>
       <c r="B40" t="n">
-        <v>272.22</v>
+        <v>136.11</v>
       </c>
       <c r="C40" t="n">
-        <v>16.72935363769534</v>
+        <v>136.11</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="n">
-        <v>228.4983978271484</v>
+        <v>0</v>
       </c>
       <c r="B41" t="n">
-        <v>242.31</v>
+        <v>94.23</v>
       </c>
       <c r="C41" t="n">
-        <v>13.81160217285156</v>
+        <v>94.23</v>
       </c>
     </row>
     <row r="42">
@@ -903,1825 +903,1693 @@
         <v>0</v>
       </c>
       <c r="B42" t="n">
-        <v>136.11</v>
+        <v>98</v>
       </c>
       <c r="C42" t="n">
-        <v>136.11</v>
+        <v>98</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="n">
-        <v>0</v>
+        <v>211.7123413085938</v>
       </c>
       <c r="B43" t="n">
-        <v>98</v>
+        <v>214.08</v>
       </c>
       <c r="C43" t="n">
-        <v>98</v>
+        <v>2.367658691406263</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="n">
-        <v>0</v>
+        <v>208.9158325195312</v>
       </c>
       <c r="B44" t="n">
-        <v>94.23</v>
+        <v>208.02</v>
       </c>
       <c r="C44" t="n">
-        <v>94.23</v>
+        <v>0.8958325195312398</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="n">
-        <v>0</v>
+        <v>210.8195495605469</v>
       </c>
       <c r="B45" t="n">
-        <v>94.23</v>
+        <v>210</v>
       </c>
       <c r="C45" t="n">
-        <v>94.23</v>
+        <v>0.819549560546875</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="n">
-        <v>211.7123413085938</v>
+        <v>218.3710174560547</v>
       </c>
       <c r="B46" t="n">
-        <v>208.02</v>
+        <v>218.32</v>
       </c>
       <c r="C46" t="n">
-        <v>3.69234130859374</v>
+        <v>0.05101745605469432</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="n">
-        <v>208.9158325195312</v>
+        <v>227.4371795654297</v>
       </c>
       <c r="B47" t="n">
-        <v>210</v>
+        <v>227.32</v>
       </c>
       <c r="C47" t="n">
-        <v>1.08416748046875</v>
+        <v>0.1171795654296943</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="n">
-        <v>210.8195495605469</v>
+        <v>241.0711212158203</v>
       </c>
       <c r="B48" t="n">
-        <v>214.08</v>
+        <v>234.57</v>
       </c>
       <c r="C48" t="n">
-        <v>3.260450439453138</v>
+        <v>6.501121215820319</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="n">
-        <v>218.3710174560547</v>
+        <v>266.0500793457031</v>
       </c>
       <c r="B49" t="n">
-        <v>218.32</v>
+        <v>256.4</v>
       </c>
       <c r="C49" t="n">
-        <v>0.05101745605469432</v>
+        <v>9.650079345703148</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="n">
-        <v>227.4371795654297</v>
+        <v>277.5600280761719</v>
       </c>
       <c r="B50" t="n">
-        <v>218.32</v>
+        <v>272.22</v>
       </c>
       <c r="C50" t="n">
-        <v>9.117179565429694</v>
+        <v>5.340028076171848</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="n">
-        <v>241.0711212158203</v>
+        <v>291.1525573730469</v>
       </c>
       <c r="B51" t="n">
-        <v>227.32</v>
+        <v>282.69</v>
       </c>
       <c r="C51" t="n">
-        <v>13.75112121582032</v>
+        <v>8.462557373046877</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="n">
-        <v>253.6593017578125</v>
+        <v>302.1669921875</v>
       </c>
       <c r="B52" t="n">
-        <v>234.57</v>
+        <v>294</v>
       </c>
       <c r="C52" t="n">
-        <v>19.08930175781251</v>
+        <v>8.1669921875</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="n">
-        <v>266.0500793457031</v>
+        <v>302.3202819824219</v>
       </c>
       <c r="B53" t="n">
-        <v>256.4</v>
+        <v>302.05</v>
       </c>
       <c r="C53" t="n">
-        <v>9.650079345703148</v>
+        <v>0.2702819824218636</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="n">
-        <v>277.5600280761719</v>
+        <v>298.3294677734375</v>
       </c>
       <c r="B54" t="n">
-        <v>272.22</v>
+        <v>302.05</v>
       </c>
       <c r="C54" t="n">
-        <v>5.340028076171848</v>
+        <v>3.720532226562511</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="n">
-        <v>291.1525573730469</v>
+        <v>278.379150390625</v>
       </c>
       <c r="B55" t="n">
-        <v>282.69</v>
+        <v>286.36</v>
       </c>
       <c r="C55" t="n">
-        <v>8.462557373046877</v>
+        <v>7.980849609375014</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="n">
-        <v>302.1669921875</v>
+        <v>254.7506713867188</v>
       </c>
       <c r="B56" t="n">
-        <v>294</v>
+        <v>265.66</v>
       </c>
       <c r="C56" t="n">
-        <v>8.1669921875</v>
+        <v>10.90932861328128</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="n">
-        <v>302.3202819824219</v>
+        <v>240.5081329345703</v>
       </c>
       <c r="B57" t="n">
-        <v>294</v>
+        <v>247.75</v>
       </c>
       <c r="C57" t="n">
-        <v>8.320281982421875</v>
+        <v>7.241867065429688</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="n">
-        <v>298.3294677734375</v>
+        <v>219.3640441894531</v>
       </c>
       <c r="B58" t="n">
-        <v>294</v>
+        <v>225</v>
       </c>
       <c r="C58" t="n">
-        <v>4.3294677734375</v>
+        <v>5.635955810546875</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="n">
-        <v>278.379150390625</v>
+        <v>205.9517822265625</v>
       </c>
       <c r="B59" t="n">
-        <v>290.13</v>
+        <v>216.18</v>
       </c>
       <c r="C59" t="n">
-        <v>11.750849609375</v>
+        <v>10.22821777343751</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="n">
-        <v>254.7506713867188</v>
+        <v>196.8549957275391</v>
       </c>
       <c r="B60" t="n">
-        <v>265.66</v>
+        <v>204.17</v>
       </c>
       <c r="C60" t="n">
-        <v>10.90932861328128</v>
+        <v>7.315004272460925</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="n">
-        <v>240.5081329345703</v>
+        <v>252.7695617675781</v>
       </c>
       <c r="B61" t="n">
-        <v>247.75</v>
+        <v>245</v>
       </c>
       <c r="C61" t="n">
-        <v>7.241867065429688</v>
+        <v>7.769561767578125</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="n">
-        <v>219.3640441894531</v>
+        <v>250.5434722900391</v>
       </c>
       <c r="B62" t="n">
-        <v>225</v>
+        <v>250.57</v>
       </c>
       <c r="C62" t="n">
-        <v>5.635955810546875</v>
+        <v>0.02652770996093068</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="n">
-        <v>205.9517822265625</v>
+        <v>245.9645080566406</v>
       </c>
       <c r="B63" t="n">
-        <v>216.18</v>
+        <v>247.75</v>
       </c>
       <c r="C63" t="n">
-        <v>10.22821777343751</v>
+        <v>1.785491943359375</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="n">
-        <v>196.8549957275391</v>
+        <v>244.8161468505859</v>
       </c>
       <c r="B64" t="n">
-        <v>204.17</v>
+        <v>245</v>
       </c>
       <c r="C64" t="n">
-        <v>7.315004272460925</v>
+        <v>0.1838531494140625</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="n">
-        <v>252.7695617675781</v>
+        <v>242.7817687988281</v>
       </c>
       <c r="B65" t="n">
         <v>245</v>
       </c>
       <c r="C65" t="n">
-        <v>7.769561767578125</v>
+        <v>2.218231201171875</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="n">
-        <v>250.5434722900391</v>
+        <v>239.2048645019531</v>
       </c>
       <c r="B66" t="n">
-        <v>245</v>
+        <v>242.31</v>
       </c>
       <c r="C66" t="n">
-        <v>5.543472290039062</v>
+        <v>3.105135498046877</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="n">
-        <v>245.9645080566406</v>
+        <v>236.3462219238281</v>
       </c>
       <c r="B67" t="n">
-        <v>245</v>
+        <v>239.67</v>
       </c>
       <c r="C67" t="n">
-        <v>0.964508056640625</v>
+        <v>3.323778076171862</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="n">
-        <v>244.8161468505859</v>
+        <v>227.77001953125</v>
       </c>
       <c r="B68" t="n">
-        <v>245</v>
+        <v>234.57</v>
       </c>
       <c r="C68" t="n">
-        <v>0.1838531494140625</v>
+        <v>6.799980468749993</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="n">
-        <v>242.7817687988281</v>
+        <v>228.4836883544922</v>
       </c>
       <c r="B69" t="n">
-        <v>245</v>
+        <v>225</v>
       </c>
       <c r="C69" t="n">
-        <v>2.218231201171875</v>
+        <v>3.483688354492188</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="n">
-        <v>239.2048645019531</v>
+        <v>241.0185699462891</v>
       </c>
       <c r="B70" t="n">
         <v>242.31</v>
       </c>
       <c r="C70" t="n">
-        <v>3.105135498046877</v>
+        <v>1.29143005371094</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="n">
-        <v>236.3462219238281</v>
+        <v>243.4589385986328</v>
       </c>
       <c r="B71" t="n">
-        <v>239.67</v>
+        <v>242.31</v>
       </c>
       <c r="C71" t="n">
-        <v>3.323778076171862</v>
+        <v>1.14893859863281</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="n">
-        <v>227.77001953125</v>
+        <v>242.0271453857422</v>
       </c>
       <c r="B72" t="n">
-        <v>239.67</v>
+        <v>245</v>
       </c>
       <c r="C72" t="n">
-        <v>11.89998046874999</v>
+        <v>2.972854614257812</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="n">
-        <v>228.4836883544922</v>
+        <v>238.9336395263672</v>
       </c>
       <c r="B73" t="n">
-        <v>239.67</v>
+        <v>242.31</v>
       </c>
       <c r="C73" t="n">
-        <v>11.1863116455078</v>
+        <v>3.376360473632815</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="n">
-        <v>241.0185699462891</v>
+        <v>233.3549041748047</v>
       </c>
       <c r="B74" t="n">
-        <v>242.31</v>
+        <v>234.57</v>
       </c>
       <c r="C74" t="n">
-        <v>1.29143005371094</v>
+        <v>1.215095825195306</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="n">
-        <v>243.4589385986328</v>
+        <v>223.5497283935547</v>
       </c>
       <c r="B75" t="n">
-        <v>242.31</v>
+        <v>232.11</v>
       </c>
       <c r="C75" t="n">
-        <v>1.14893859863281</v>
+        <v>8.560271606445326</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="n">
-        <v>242.0271453857422</v>
+        <v>213.1903228759766</v>
       </c>
       <c r="B76" t="n">
-        <v>242.31</v>
+        <v>220.5</v>
       </c>
       <c r="C76" t="n">
-        <v>0.2828546142578148</v>
+        <v>7.309677124023438</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="n">
-        <v>238.9336395263672</v>
+        <v>197.3602294921875</v>
       </c>
       <c r="B77" t="n">
-        <v>242.31</v>
+        <v>204.17</v>
       </c>
       <c r="C77" t="n">
-        <v>3.376360473632815</v>
+        <v>6.809770507812487</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="n">
-        <v>233.3549041748047</v>
+        <v>355.5089111328125</v>
       </c>
       <c r="B78" t="n">
-        <v>237.1</v>
+        <v>188.46</v>
       </c>
       <c r="C78" t="n">
-        <v>3.745095825195307</v>
+        <v>167.0489111328125</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="n">
-        <v>223.5497283935547</v>
+        <v>343.0353698730469</v>
       </c>
       <c r="B79" t="n">
-        <v>232.11</v>
+        <v>159.78</v>
       </c>
       <c r="C79" t="n">
-        <v>8.560271606445326</v>
+        <v>183.2553698730469</v>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="n">
-        <v>213.1903228759766</v>
+        <v>332.6474914550781</v>
       </c>
       <c r="B80" t="n">
-        <v>218.32</v>
+        <v>124.58</v>
       </c>
       <c r="C80" t="n">
-        <v>5.129677124023431</v>
+        <v>208.0674914550781</v>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="n">
-        <v>197.3602294921875</v>
+        <v>239.928955078125</v>
       </c>
       <c r="B81" t="n">
-        <v>204.17</v>
+        <v>239.67</v>
       </c>
       <c r="C81" t="n">
-        <v>6.809770507812487</v>
+        <v>0.2589550781250125</v>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="n">
-        <v>355.5089111328125</v>
+        <v>232.9545440673828</v>
       </c>
       <c r="B82" t="n">
-        <v>188.46</v>
+        <v>237.1</v>
       </c>
       <c r="C82" t="n">
-        <v>167.0489111328125</v>
+        <v>4.145455932617182</v>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="n">
-        <v>343.0353698730469</v>
+        <v>223.3844451904297</v>
       </c>
       <c r="B83" t="n">
-        <v>159.78</v>
+        <v>227.32</v>
       </c>
       <c r="C83" t="n">
-        <v>183.2553698730469</v>
+        <v>3.935554809570306</v>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="n">
-        <v>332.6474914550781</v>
+        <v>218.9897308349609</v>
       </c>
       <c r="B84" t="n">
-        <v>124.58</v>
+        <v>222.73</v>
       </c>
       <c r="C84" t="n">
-        <v>208.0674914550781</v>
+        <v>3.740269165039052</v>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="n">
-        <v>239.928955078125</v>
+        <v>215.0123901367188</v>
       </c>
       <c r="B85" t="n">
-        <v>227.32</v>
+        <v>218.32</v>
       </c>
       <c r="C85" t="n">
-        <v>12.60895507812501</v>
+        <v>3.307609863281243</v>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="n">
-        <v>232.9545440673828</v>
+        <v>210.9894256591797</v>
       </c>
       <c r="B86" t="n">
-        <v>227.32</v>
+        <v>210</v>
       </c>
       <c r="C86" t="n">
-        <v>5.634544067382819</v>
+        <v>0.9894256591796875</v>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="n">
-        <v>223.3844451904297</v>
+        <v>215.0703277587891</v>
       </c>
       <c r="B87" t="n">
-        <v>227.32</v>
+        <v>212.02</v>
       </c>
       <c r="C87" t="n">
-        <v>3.935554809570306</v>
+        <v>3.050327758789052</v>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="n">
-        <v>218.9897308349609</v>
+        <v>223.0034790039062</v>
       </c>
       <c r="B88" t="n">
-        <v>222.73</v>
+        <v>216.18</v>
       </c>
       <c r="C88" t="n">
-        <v>3.740269165039052</v>
+        <v>6.823479003906243</v>
       </c>
     </row>
     <row r="89">
       <c r="A89" t="n">
-        <v>215.0123901367188</v>
+        <v>245.0893096923828</v>
       </c>
       <c r="B89" t="n">
-        <v>218.32</v>
+        <v>237.1</v>
       </c>
       <c r="C89" t="n">
-        <v>3.307609863281243</v>
+        <v>7.989309692382818</v>
       </c>
     </row>
     <row r="90">
       <c r="A90" t="n">
-        <v>208.926025390625</v>
+        <v>266.6002197265625</v>
       </c>
       <c r="B90" t="n">
-        <v>216.18</v>
+        <v>247.75</v>
       </c>
       <c r="C90" t="n">
-        <v>7.253974609375007</v>
+        <v>18.8502197265625</v>
       </c>
     </row>
     <row r="91">
       <c r="A91" t="n">
-        <v>210.9894256591797</v>
+        <v>305.3719177246094</v>
       </c>
       <c r="B91" t="n">
-        <v>216.18</v>
+        <v>294</v>
       </c>
       <c r="C91" t="n">
-        <v>5.190574340820319</v>
+        <v>11.37191772460938</v>
       </c>
     </row>
     <row r="92">
       <c r="A92" t="n">
-        <v>215.0703277587891</v>
+        <v>313.0787048339844</v>
       </c>
       <c r="B92" t="n">
-        <v>210</v>
+        <v>306.25</v>
       </c>
       <c r="C92" t="n">
-        <v>5.070327758789062</v>
+        <v>6.828704833984375</v>
       </c>
     </row>
     <row r="93">
       <c r="A93" t="n">
-        <v>223.0034790039062</v>
+        <v>318.2262268066406</v>
       </c>
       <c r="B93" t="n">
-        <v>210</v>
+        <v>315</v>
       </c>
       <c r="C93" t="n">
-        <v>13.00347900390625</v>
+        <v>3.226226806640625</v>
       </c>
     </row>
     <row r="94">
       <c r="A94" t="n">
-        <v>294.8748168945312</v>
+        <v>321.3894958496094</v>
       </c>
       <c r="B94" t="n">
-        <v>237.1</v>
+        <v>319.57</v>
       </c>
       <c r="C94" t="n">
-        <v>57.77481689453126</v>
+        <v>1.819495849609382</v>
       </c>
     </row>
     <row r="95">
       <c r="A95" t="n">
-        <v>305.3719177246094</v>
+        <v>321.5060729980469</v>
       </c>
       <c r="B95" t="n">
-        <v>294</v>
+        <v>324.26</v>
       </c>
       <c r="C95" t="n">
-        <v>11.37191772460938</v>
+        <v>2.753927001953116</v>
       </c>
     </row>
     <row r="96">
       <c r="A96" t="n">
-        <v>313.0787048339844</v>
+        <v>318.923828125</v>
       </c>
       <c r="B96" t="n">
-        <v>306.25</v>
+        <v>324.26</v>
       </c>
       <c r="C96" t="n">
-        <v>6.828704833984375</v>
+        <v>5.336171874999991</v>
       </c>
     </row>
     <row r="97">
       <c r="A97" t="n">
-        <v>318.2262268066406</v>
+        <v>315.6445922851562</v>
       </c>
       <c r="B97" t="n">
-        <v>315</v>
+        <v>319.57</v>
       </c>
       <c r="C97" t="n">
-        <v>3.226226806640625</v>
+        <v>3.925407714843743</v>
       </c>
     </row>
     <row r="98">
       <c r="A98" t="n">
-        <v>321.3894958496094</v>
+        <v>310.4517517089844</v>
       </c>
       <c r="B98" t="n">
-        <v>319.57</v>
+        <v>315</v>
       </c>
       <c r="C98" t="n">
-        <v>1.819495849609382</v>
+        <v>4.548248291015625</v>
       </c>
     </row>
     <row r="99">
       <c r="A99" t="n">
-        <v>321.5060729980469</v>
+        <v>306.2401733398438</v>
       </c>
       <c r="B99" t="n">
-        <v>319.57</v>
+        <v>310.56</v>
       </c>
       <c r="C99" t="n">
-        <v>1.936072998046882</v>
+        <v>4.319826660156252</v>
       </c>
     </row>
     <row r="100">
       <c r="A100" t="n">
-        <v>318.923828125</v>
+        <v>307.2374877929688</v>
       </c>
       <c r="B100" t="n">
-        <v>319.57</v>
+        <v>306.25</v>
       </c>
       <c r="C100" t="n">
-        <v>0.6461718749999932</v>
+        <v>0.98748779296875</v>
       </c>
     </row>
     <row r="101">
       <c r="A101" t="n">
-        <v>315.6445922851562</v>
+        <v>306.7879333496094</v>
       </c>
       <c r="B101" t="n">
-        <v>319.57</v>
+        <v>306.25</v>
       </c>
       <c r="C101" t="n">
-        <v>3.925407714843743</v>
+        <v>0.537933349609375</v>
       </c>
     </row>
     <row r="102">
       <c r="A102" t="n">
-        <v>310.4517517089844</v>
+        <v>307.1228942871094</v>
       </c>
       <c r="B102" t="n">
-        <v>315</v>
+        <v>306.25</v>
       </c>
       <c r="C102" t="n">
-        <v>4.548248291015625</v>
+        <v>0.872894287109375</v>
       </c>
     </row>
     <row r="103">
       <c r="A103" t="n">
-        <v>306.2401733398438</v>
+        <v>309.24853515625</v>
       </c>
       <c r="B103" t="n">
-        <v>310.56</v>
+        <v>306.25</v>
       </c>
       <c r="C103" t="n">
-        <v>4.319826660156252</v>
+        <v>2.99853515625</v>
       </c>
     </row>
     <row r="104">
       <c r="A104" t="n">
-        <v>307.2374877929688</v>
+        <v>309.5013122558594</v>
       </c>
       <c r="B104" t="n">
-        <v>306.25</v>
+        <v>310.56</v>
       </c>
       <c r="C104" t="n">
-        <v>0.98748779296875</v>
+        <v>1.058687744140627</v>
       </c>
     </row>
     <row r="105">
       <c r="A105" t="n">
-        <v>306.7879333496094</v>
+        <v>307.8377685546875</v>
       </c>
       <c r="B105" t="n">
-        <v>306.25</v>
+        <v>310.56</v>
       </c>
       <c r="C105" t="n">
-        <v>0.537933349609375</v>
+        <v>2.722231445312502</v>
       </c>
     </row>
     <row r="106">
       <c r="A106" t="n">
-        <v>307.1228942871094</v>
+        <v>305.3421020507812</v>
       </c>
       <c r="B106" t="n">
         <v>306.25</v>
       </c>
       <c r="C106" t="n">
-        <v>0.872894287109375</v>
+        <v>0.90789794921875</v>
       </c>
     </row>
     <row r="107">
       <c r="A107" t="n">
-        <v>309.24853515625</v>
+        <v>302.3069763183594</v>
       </c>
       <c r="B107" t="n">
         <v>306.25</v>
       </c>
       <c r="C107" t="n">
-        <v>2.99853515625</v>
+        <v>3.943023681640625</v>
       </c>
     </row>
     <row r="108">
       <c r="A108" t="n">
-        <v>309.5013122558594</v>
+        <v>298.0066528320312</v>
       </c>
       <c r="B108" t="n">
-        <v>306.25</v>
+        <v>302.05</v>
       </c>
       <c r="C108" t="n">
-        <v>3.251312255859375</v>
+        <v>4.043347167968761</v>
       </c>
     </row>
     <row r="109">
       <c r="A109" t="n">
-        <v>307.8377685546875</v>
+        <v>277.2246704101562</v>
       </c>
       <c r="B109" t="n">
-        <v>306.25</v>
+        <v>297.97</v>
       </c>
       <c r="C109" t="n">
-        <v>1.5877685546875</v>
+        <v>20.74532958984378</v>
       </c>
     </row>
     <row r="110">
       <c r="A110" t="n">
-        <v>305.3421020507812</v>
+        <v>267.5450134277344</v>
       </c>
       <c r="B110" t="n">
-        <v>306.25</v>
+        <v>286.36</v>
       </c>
       <c r="C110" t="n">
-        <v>0.90789794921875</v>
+        <v>18.81498657226564</v>
       </c>
     </row>
     <row r="111">
       <c r="A111" t="n">
-        <v>302.3069763183594</v>
+        <v>268.3763732910156</v>
       </c>
       <c r="B111" t="n">
-        <v>306.25</v>
+        <v>268.9</v>
       </c>
       <c r="C111" t="n">
-        <v>3.943023681640625</v>
+        <v>0.5236267089843523</v>
       </c>
     </row>
     <row r="112">
       <c r="A112" t="n">
-        <v>298.0066528320312</v>
+        <v>268.1117858886719</v>
       </c>
       <c r="B112" t="n">
-        <v>302.05</v>
+        <v>265.66</v>
       </c>
       <c r="C112" t="n">
-        <v>4.043347167968761</v>
+        <v>2.45178588867185</v>
       </c>
     </row>
     <row r="113">
       <c r="A113" t="n">
-        <v>277.2246704101562</v>
+        <v>273.9475708007812</v>
       </c>
       <c r="B113" t="n">
-        <v>297.97</v>
+        <v>268.9</v>
       </c>
       <c r="C113" t="n">
-        <v>20.74532958984378</v>
+        <v>5.047570800781273</v>
       </c>
     </row>
     <row r="114">
       <c r="A114" t="n">
-        <v>267.5450134277344</v>
+        <v>283.0668334960938</v>
       </c>
       <c r="B114" t="n">
-        <v>290.13</v>
+        <v>275.62</v>
       </c>
       <c r="C114" t="n">
-        <v>22.58498657226562</v>
+        <v>7.446833496093745</v>
       </c>
     </row>
     <row r="115">
       <c r="A115" t="n">
-        <v>268.3763732910156</v>
+        <v>282.9918823242188</v>
       </c>
       <c r="B115" t="n">
-        <v>268.9</v>
+        <v>286.36</v>
       </c>
       <c r="C115" t="n">
-        <v>0.5236267089843523</v>
+        <v>3.368117675781264</v>
       </c>
     </row>
     <row r="116">
       <c r="A116" t="n">
-        <v>268.1117858886719</v>
+        <v>268.4938659667969</v>
       </c>
       <c r="B116" t="n">
-        <v>268.9</v>
+        <v>282.69</v>
       </c>
       <c r="C116" t="n">
-        <v>0.7882141113281023</v>
+        <v>14.19613403320312</v>
       </c>
     </row>
     <row r="117">
       <c r="A117" t="n">
-        <v>273.9475708007812</v>
+        <v>247.6003570556641</v>
       </c>
       <c r="B117" t="n">
-        <v>268.9</v>
+        <v>259.41</v>
       </c>
       <c r="C117" t="n">
-        <v>5.047570800781273</v>
+        <v>11.80964294433596</v>
       </c>
     </row>
     <row r="118">
       <c r="A118" t="n">
-        <v>283.0668334960938</v>
+        <v>0</v>
       </c>
       <c r="B118" t="n">
-        <v>275.62</v>
+        <v>262.5</v>
       </c>
       <c r="C118" t="n">
-        <v>7.446833496093745</v>
+        <v>262.5</v>
       </c>
     </row>
     <row r="119">
       <c r="A119" t="n">
-        <v>282.9918823242188</v>
+        <v>0</v>
       </c>
       <c r="B119" t="n">
-        <v>275.62</v>
+        <v>143.18</v>
       </c>
       <c r="C119" t="n">
-        <v>7.371882324218745</v>
+        <v>143.18</v>
       </c>
     </row>
     <row r="120">
       <c r="A120" t="n">
-        <v>268.4938659667969</v>
+        <v>238.3794860839844</v>
       </c>
       <c r="B120" t="n">
-        <v>275.62</v>
+        <v>214.08</v>
       </c>
       <c r="C120" t="n">
-        <v>7.12613403320313</v>
+        <v>24.29948608398436</v>
       </c>
     </row>
     <row r="121">
       <c r="A121" t="n">
-        <v>247.6003570556641</v>
+        <v>240.141357421875</v>
       </c>
       <c r="B121" t="n">
-        <v>262.5</v>
+        <v>239.67</v>
       </c>
       <c r="C121" t="n">
-        <v>14.89964294433594</v>
+        <v>0.4713574218750125</v>
       </c>
     </row>
     <row r="122">
       <c r="A122" t="n">
-        <v>0</v>
+        <v>240.7535247802734</v>
       </c>
       <c r="B122" t="n">
-        <v>259.41</v>
+        <v>239.67</v>
       </c>
       <c r="C122" t="n">
-        <v>259.41</v>
+        <v>1.08352478027345</v>
       </c>
     </row>
     <row r="123">
       <c r="A123" t="n">
-        <v>0</v>
+        <v>243.9438323974609</v>
       </c>
       <c r="B123" t="n">
-        <v>214.08</v>
+        <v>239.67</v>
       </c>
       <c r="C123" t="n">
-        <v>214.08</v>
+        <v>4.27383239746095</v>
       </c>
     </row>
     <row r="124">
       <c r="A124" t="n">
-        <v>0</v>
+        <v>249.35498046875</v>
       </c>
       <c r="B124" t="n">
-        <v>214.08</v>
+        <v>245</v>
       </c>
       <c r="C124" t="n">
-        <v>214.08</v>
+        <v>4.35498046875</v>
       </c>
     </row>
     <row r="125">
       <c r="A125" t="n">
-        <v>238.3794860839844</v>
+        <v>250.5413513183594</v>
       </c>
       <c r="B125" t="n">
-        <v>214.08</v>
+        <v>250.57</v>
       </c>
       <c r="C125" t="n">
-        <v>24.29948608398436</v>
+        <v>0.02864868164061818</v>
       </c>
     </row>
     <row r="126">
       <c r="A126" t="n">
-        <v>240.141357421875</v>
+        <v>246.8910217285156</v>
       </c>
       <c r="B126" t="n">
-        <v>239.67</v>
+        <v>250.57</v>
       </c>
       <c r="C126" t="n">
-        <v>0.4713574218750125</v>
+        <v>3.678978271484368</v>
       </c>
     </row>
     <row r="127">
       <c r="A127" t="n">
-        <v>240.7535247802734</v>
+        <v>219.9246215820312</v>
       </c>
       <c r="B127" t="n">
-        <v>239.67</v>
+        <v>234.57</v>
       </c>
       <c r="C127" t="n">
-        <v>1.08352478027345</v>
+        <v>14.64537841796874</v>
       </c>
     </row>
     <row r="128">
       <c r="A128" t="n">
-        <v>243.9438323974609</v>
+        <v>231.4132690429688</v>
       </c>
       <c r="B128" t="n">
         <v>239.67</v>
       </c>
       <c r="C128" t="n">
-        <v>4.27383239746095</v>
+        <v>8.256730957031237</v>
       </c>
     </row>
     <row r="129">
       <c r="A129" t="n">
-        <v>249.35498046875</v>
+        <v>224.3855438232422</v>
       </c>
       <c r="B129" t="n">
-        <v>245</v>
+        <v>232.11</v>
       </c>
       <c r="C129" t="n">
-        <v>4.35498046875</v>
+        <v>7.724456176757826</v>
       </c>
     </row>
     <row r="130">
       <c r="A130" t="n">
-        <v>250.5413513183594</v>
+        <v>219.9381256103516</v>
       </c>
       <c r="B130" t="n">
-        <v>245</v>
+        <v>220.5</v>
       </c>
       <c r="C130" t="n">
-        <v>5.541351318359375</v>
+        <v>0.5618743896484375</v>
       </c>
     </row>
     <row r="131">
       <c r="A131" t="n">
-        <v>246.8910217285156</v>
+        <v>216.3335876464844</v>
       </c>
       <c r="B131" t="n">
-        <v>245</v>
+        <v>218.32</v>
       </c>
       <c r="C131" t="n">
-        <v>1.891021728515625</v>
+        <v>1.986412353515618</v>
       </c>
     </row>
     <row r="132">
       <c r="A132" t="n">
-        <v>219.9246215820312</v>
+        <v>213.7152252197266</v>
       </c>
       <c r="B132" t="n">
-        <v>239.67</v>
+        <v>216.18</v>
       </c>
       <c r="C132" t="n">
-        <v>19.74537841796874</v>
+        <v>2.464774780273444</v>
       </c>
     </row>
     <row r="133">
       <c r="A133" t="n">
-        <v>240.9544830322266</v>
+        <v>222.2797698974609</v>
       </c>
       <c r="B133" t="n">
-        <v>234.57</v>
+        <v>216.18</v>
       </c>
       <c r="C133" t="n">
-        <v>6.384483032226569</v>
+        <v>6.099769897460931</v>
       </c>
     </row>
     <row r="134">
       <c r="A134" t="n">
-        <v>231.4132690429688</v>
+        <v>272.3433837890625</v>
       </c>
       <c r="B134" t="n">
-        <v>232.11</v>
+        <v>275.62</v>
       </c>
       <c r="C134" t="n">
-        <v>0.6967309570312636</v>
+        <v>3.276616210937505</v>
       </c>
     </row>
     <row r="135">
       <c r="A135" t="n">
-        <v>224.3855438232422</v>
+        <v>281.0038452148438</v>
       </c>
       <c r="B135" t="n">
-        <v>220.5</v>
+        <v>290.13</v>
       </c>
       <c r="C135" t="n">
-        <v>3.885543823242188</v>
+        <v>9.126154785156245</v>
       </c>
     </row>
     <row r="136">
       <c r="A136" t="n">
-        <v>219.9381256103516</v>
+        <v>244.625244140625</v>
       </c>
       <c r="B136" t="n">
-        <v>220.5</v>
+        <v>268.9</v>
       </c>
       <c r="C136" t="n">
-        <v>0.5618743896484375</v>
+        <v>24.27475585937498</v>
       </c>
     </row>
     <row r="137">
       <c r="A137" t="n">
-        <v>216.3335876464844</v>
+        <v>230.6876983642578</v>
       </c>
       <c r="B137" t="n">
-        <v>218.32</v>
+        <v>250.57</v>
       </c>
       <c r="C137" t="n">
-        <v>1.986412353515618</v>
+        <v>19.88230163574218</v>
       </c>
     </row>
     <row r="138">
       <c r="A138" t="n">
-        <v>213.7152252197266</v>
+        <v>218.7195892333984</v>
       </c>
       <c r="B138" t="n">
-        <v>218.32</v>
+        <v>225</v>
       </c>
       <c r="C138" t="n">
-        <v>4.604774780273431</v>
+        <v>6.280410766601562</v>
       </c>
     </row>
     <row r="139">
       <c r="A139" t="n">
-        <v>222.2797698974609</v>
+        <v>181.3059997558594</v>
       </c>
       <c r="B139" t="n">
-        <v>216.18</v>
+        <v>183.75</v>
       </c>
       <c r="C139" t="n">
-        <v>6.099769897460931</v>
+        <v>2.444000244140625</v>
       </c>
     </row>
     <row r="140">
       <c r="A140" t="n">
-        <v>238.4279174804688</v>
+        <v>183.3445739746094</v>
       </c>
       <c r="B140" t="n">
-        <v>216.18</v>
+        <v>180.74</v>
       </c>
       <c r="C140" t="n">
-        <v>22.24791748046874</v>
+        <v>2.604573974609366</v>
       </c>
     </row>
     <row r="141">
       <c r="A141" t="n">
-        <v>257.7305603027344</v>
+        <v>188.4166259765625</v>
       </c>
       <c r="B141" t="n">
-        <v>216.18</v>
+        <v>183.75</v>
       </c>
       <c r="C141" t="n">
-        <v>41.55056030273437</v>
+        <v>4.6666259765625</v>
       </c>
     </row>
     <row r="142">
       <c r="A142" t="n">
-        <v>295.9156494140625</v>
+        <v>196.8783264160156</v>
       </c>
       <c r="B142" t="n">
-        <v>268.9</v>
+        <v>188.46</v>
       </c>
       <c r="C142" t="n">
-        <v>27.01564941406252</v>
+        <v>8.418326416015617</v>
       </c>
     </row>
     <row r="143">
       <c r="A143" t="n">
-        <v>281.0038452148438</v>
+        <v>207.0765075683594</v>
       </c>
       <c r="B143" t="n">
-        <v>250.57</v>
+        <v>195.13</v>
       </c>
       <c r="C143" t="n">
-        <v>30.43384521484376</v>
+        <v>11.94650756835938</v>
       </c>
     </row>
     <row r="144">
       <c r="A144" t="n">
-        <v>244.625244140625</v>
+        <v>207.0622100830078</v>
       </c>
       <c r="B144" t="n">
-        <v>268.9</v>
+        <v>206.07</v>
       </c>
       <c r="C144" t="n">
-        <v>24.27475585937498</v>
+        <v>0.9922100830078193</v>
       </c>
     </row>
     <row r="145">
       <c r="A145" t="n">
-        <v>230.6876983642578</v>
+        <v>205.270751953125</v>
       </c>
       <c r="B145" t="n">
-        <v>268.9</v>
+        <v>204.17</v>
       </c>
       <c r="C145" t="n">
-        <v>38.21230163574216</v>
+        <v>1.100751953125013</v>
       </c>
     </row>
     <row r="146">
       <c r="A146" t="n">
-        <v>218.7195892333984</v>
+        <v>203.6882476806641</v>
       </c>
       <c r="B146" t="n">
-        <v>250.57</v>
+        <v>206.07</v>
       </c>
       <c r="C146" t="n">
-        <v>31.85041076660156</v>
+        <v>2.381752319335931</v>
       </c>
     </row>
     <row r="147">
       <c r="A147" t="n">
-        <v>193.02001953125</v>
+        <v>201.5074615478516</v>
       </c>
       <c r="B147" t="n">
-        <v>193.42</v>
+        <v>206.07</v>
       </c>
       <c r="C147" t="n">
-        <v>0.3999804687499875</v>
+        <v>4.562538452148431</v>
       </c>
     </row>
     <row r="148">
       <c r="A148" t="n">
-        <v>184.2410278320312</v>
+        <v>196.6033630371094</v>
       </c>
       <c r="B148" t="n">
-        <v>180.74</v>
+        <v>204.17</v>
       </c>
       <c r="C148" t="n">
-        <v>3.501027832031241</v>
+        <v>7.566636962890612</v>
       </c>
     </row>
     <row r="149">
       <c r="A149" t="n">
-        <v>207.0622100830078</v>
+        <v>190.1020202636719</v>
       </c>
       <c r="B149" t="n">
-        <v>195.13</v>
+        <v>198.65</v>
       </c>
       <c r="C149" t="n">
-        <v>11.93221008300782</v>
+        <v>8.547979736328131</v>
       </c>
     </row>
     <row r="150">
       <c r="A150" t="n">
-        <v>205.270751953125</v>
+        <v>185.960205078125</v>
       </c>
       <c r="B150" t="n">
-        <v>204.17</v>
+        <v>190.09</v>
       </c>
       <c r="C150" t="n">
-        <v>1.100751953125013</v>
+        <v>4.129794921875003</v>
       </c>
     </row>
     <row r="151">
       <c r="A151" t="n">
-        <v>203.6882476806641</v>
+        <v>180.1084289550781</v>
       </c>
       <c r="B151" t="n">
-        <v>206.07</v>
+        <v>188.46</v>
       </c>
       <c r="C151" t="n">
-        <v>2.381752319335931</v>
+        <v>8.351571044921883</v>
       </c>
     </row>
     <row r="152">
       <c r="A152" t="n">
-        <v>201.5074615478516</v>
+        <v>226.7194671630859</v>
       </c>
       <c r="B152" t="n">
-        <v>206.07</v>
+        <v>232.11</v>
       </c>
       <c r="C152" t="n">
-        <v>4.562538452148431</v>
+        <v>5.390532836914076</v>
       </c>
     </row>
     <row r="153">
       <c r="A153" t="n">
-        <v>196.6033630371094</v>
+        <v>218.0660095214844</v>
       </c>
       <c r="B153" t="n">
-        <v>206.07</v>
+        <v>225</v>
       </c>
       <c r="C153" t="n">
-        <v>9.466636962890618</v>
+        <v>6.933990478515625</v>
       </c>
     </row>
     <row r="154">
       <c r="A154" t="n">
-        <v>190.1020202636719</v>
+        <v>211.7289886474609</v>
       </c>
       <c r="B154" t="n">
-        <v>198.65</v>
+        <v>218.32</v>
       </c>
       <c r="C154" t="n">
-        <v>8.547979736328131</v>
+        <v>6.591011352539056</v>
       </c>
     </row>
     <row r="155">
       <c r="A155" t="n">
-        <v>185.960205078125</v>
+        <v>207.0608978271484</v>
       </c>
       <c r="B155" t="n">
-        <v>190.09</v>
+        <v>212.02</v>
       </c>
       <c r="C155" t="n">
-        <v>4.129794921875003</v>
+        <v>4.959102172851573</v>
       </c>
     </row>
     <row r="156">
       <c r="A156" t="n">
-        <v>180.1084289550781</v>
+        <v>204.2452697753906</v>
       </c>
       <c r="B156" t="n">
-        <v>188.46</v>
+        <v>206.07</v>
       </c>
       <c r="C156" t="n">
-        <v>8.351571044921883</v>
+        <v>1.824730224609368</v>
       </c>
     </row>
     <row r="157">
       <c r="A157" t="n">
-        <v>226.7194671630859</v>
+        <v>200.3761749267578</v>
       </c>
       <c r="B157" t="n">
-        <v>218.32</v>
+        <v>202.29</v>
       </c>
       <c r="C157" t="n">
-        <v>8.399467163085944</v>
+        <v>1.91382507324218</v>
       </c>
     </row>
     <row r="158">
       <c r="A158" t="n">
-        <v>218.0660095214844</v>
+        <v>198.5787811279297</v>
       </c>
       <c r="B158" t="n">
-        <v>218.32</v>
+        <v>202.29</v>
       </c>
       <c r="C158" t="n">
-        <v>0.2539904785156182</v>
+        <v>3.711218872070305</v>
       </c>
     </row>
     <row r="159">
       <c r="A159" t="n">
-        <v>211.7289886474609</v>
+        <v>195.5976409912109</v>
       </c>
       <c r="B159" t="n">
-        <v>218.32</v>
+        <v>200.45</v>
       </c>
       <c r="C159" t="n">
-        <v>6.591011352539056</v>
+        <v>4.852359008789051</v>
       </c>
     </row>
     <row r="160">
       <c r="A160" t="n">
-        <v>207.0608978271484</v>
+        <v>194.4798126220703</v>
       </c>
       <c r="B160" t="n">
-        <v>212.02</v>
+        <v>202.29</v>
       </c>
       <c r="C160" t="n">
-        <v>4.959102172851573</v>
+        <v>7.81018737792968</v>
       </c>
     </row>
     <row r="161">
       <c r="A161" t="n">
-        <v>204.2452697753906</v>
+        <v>190.9214782714844</v>
       </c>
       <c r="B161" t="n">
-        <v>206.07</v>
+        <v>196.88</v>
       </c>
       <c r="C161" t="n">
-        <v>1.824730224609368</v>
+        <v>5.95852172851562</v>
       </c>
     </row>
     <row r="162">
       <c r="A162" t="n">
-        <v>200.3761749267578</v>
+        <v>189.4687194824219</v>
       </c>
       <c r="B162" t="n">
-        <v>202.29</v>
+        <v>190.09</v>
       </c>
       <c r="C162" t="n">
-        <v>1.91382507324218</v>
+        <v>0.6212805175781284</v>
       </c>
     </row>
     <row r="163">
       <c r="A163" t="n">
-        <v>200.4162902832031</v>
+        <v>190.0959167480469</v>
       </c>
       <c r="B163" t="n">
-        <v>200.45</v>
+        <v>193.42</v>
       </c>
       <c r="C163" t="n">
-        <v>0.03370971679686363</v>
+        <v>3.324083251953112</v>
       </c>
     </row>
     <row r="164">
       <c r="A164" t="n">
-        <v>198.5787811279297</v>
+        <v>207.6795654296875</v>
       </c>
       <c r="B164" t="n">
-        <v>200.45</v>
+        <v>193.42</v>
       </c>
       <c r="C164" t="n">
-        <v>1.871218872070301</v>
+        <v>14.25956542968751</v>
       </c>
     </row>
     <row r="165">
       <c r="A165" t="n">
-        <v>194.4798126220703</v>
+        <v>216.7383422851562</v>
       </c>
       <c r="B165" t="n">
-        <v>190.09</v>
+        <v>204.17</v>
       </c>
       <c r="C165" t="n">
-        <v>4.389812622070309</v>
+        <v>12.56834228515626</v>
       </c>
     </row>
     <row r="166">
       <c r="A166" t="n">
-        <v>190.9214782714844</v>
+        <v>225.0151672363281</v>
       </c>
       <c r="B166" t="n">
-        <v>193.42</v>
+        <v>218.32</v>
       </c>
       <c r="C166" t="n">
-        <v>2.498521728515612</v>
+        <v>6.695167236328132</v>
       </c>
     </row>
     <row r="167">
       <c r="A167" t="n">
-        <v>189.4687194824219</v>
+        <v>232.4953308105469</v>
       </c>
       <c r="B167" t="n">
-        <v>193.42</v>
+        <v>225</v>
       </c>
       <c r="C167" t="n">
-        <v>3.951280517578112</v>
+        <v>7.495330810546875</v>
       </c>
     </row>
     <row r="168">
       <c r="A168" t="n">
-        <v>190.0959167480469</v>
+        <v>236.8334350585938</v>
       </c>
       <c r="B168" t="n">
-        <v>193.42</v>
+        <v>234.57</v>
       </c>
       <c r="C168" t="n">
-        <v>3.324083251953112</v>
+        <v>2.263435058593757</v>
       </c>
     </row>
     <row r="169">
       <c r="A169" t="n">
-        <v>207.6795654296875</v>
+        <v>232.9726104736328</v>
       </c>
       <c r="B169" t="n">
-        <v>193.42</v>
+        <v>237.1</v>
       </c>
       <c r="C169" t="n">
-        <v>14.25956542968751</v>
+        <v>4.127389526367182</v>
       </c>
     </row>
     <row r="170">
       <c r="A170" t="n">
-        <v>216.7383422851562</v>
+        <v>325.2226257324219</v>
       </c>
       <c r="B170" t="n">
-        <v>206.07</v>
+        <v>319.57</v>
       </c>
       <c r="C170" t="n">
-        <v>10.66834228515626</v>
+        <v>5.652625732421882</v>
       </c>
     </row>
     <row r="171">
       <c r="A171" t="n">
-        <v>225.0151672363281</v>
+        <v>334.8286437988281</v>
       </c>
       <c r="B171" t="n">
-        <v>218.32</v>
+        <v>319.57</v>
       </c>
       <c r="C171" t="n">
-        <v>6.695167236328132</v>
+        <v>15.25864379882813</v>
       </c>
     </row>
     <row r="172">
       <c r="A172" t="n">
-        <v>232.4953308105469</v>
+        <v>347.3280944824219</v>
       </c>
       <c r="B172" t="n">
-        <v>225</v>
+        <v>329.1</v>
       </c>
       <c r="C172" t="n">
-        <v>7.495330810546875</v>
+        <v>18.22809448242185</v>
       </c>
     </row>
     <row r="173">
       <c r="A173" t="n">
-        <v>236.8334350585938</v>
+        <v>181.6701812744141</v>
       </c>
       <c r="B173" t="n">
-        <v>225</v>
+        <v>350</v>
       </c>
       <c r="C173" t="n">
-        <v>11.83343505859375</v>
+        <v>168.3298187255859</v>
       </c>
     </row>
     <row r="174">
       <c r="A174" t="n">
-        <v>232.9726104736328</v>
+        <v>187.1005706787109</v>
       </c>
       <c r="B174" t="n">
-        <v>234.57</v>
+        <v>361.48</v>
       </c>
       <c r="C174" t="n">
-        <v>1.597389526367181</v>
+        <v>174.3794293212891</v>
       </c>
     </row>
     <row r="175">
       <c r="A175" t="n">
-        <v>228.5069427490234</v>
+        <v>190.4427642822266</v>
       </c>
       <c r="B175" t="n">
-        <v>237.1</v>
+        <v>380.17</v>
       </c>
       <c r="C175" t="n">
-        <v>8.593057250976557</v>
+        <v>189.7272357177735</v>
       </c>
     </row>
     <row r="176">
       <c r="A176" t="n">
-        <v>325.2226257324219</v>
+        <v>178.2145538330078</v>
       </c>
       <c r="B176" t="n">
-        <v>319.57</v>
+        <v>386.84</v>
       </c>
       <c r="C176" t="n">
-        <v>5.652625732421882</v>
+        <v>208.6254461669922</v>
       </c>
     </row>
     <row r="177">
       <c r="A177" t="n">
-        <v>334.8286437988281</v>
+        <v>261.30224609375</v>
       </c>
       <c r="B177" t="n">
-        <v>319.57</v>
+        <v>279.11</v>
       </c>
       <c r="C177" t="n">
-        <v>15.25864379882813</v>
+        <v>17.80775390625001</v>
       </c>
     </row>
     <row r="178">
       <c r="A178" t="n">
-        <v>347.3280944824219</v>
+        <v>248.8310699462891</v>
       </c>
       <c r="B178" t="n">
-        <v>329.1</v>
+        <v>265.66</v>
       </c>
       <c r="C178" t="n">
-        <v>18.22809448242185</v>
+        <v>16.82893005371096</v>
       </c>
     </row>
     <row r="179">
       <c r="A179" t="n">
-        <v>181.6701812744141</v>
+        <v>240.1075897216797</v>
       </c>
       <c r="B179" t="n">
-        <v>350</v>
+        <v>247.75</v>
       </c>
       <c r="C179" t="n">
-        <v>168.3298187255859</v>
+        <v>7.642410278320312</v>
       </c>
     </row>
     <row r="180">
       <c r="A180" t="n">
-        <v>187.1005706787109</v>
+        <v>233.3475952148438</v>
       </c>
       <c r="B180" t="n">
-        <v>361.48</v>
+        <v>242.31</v>
       </c>
       <c r="C180" t="n">
-        <v>174.3794293212891</v>
+        <v>8.962404785156252</v>
       </c>
     </row>
     <row r="181">
       <c r="A181" t="n">
-        <v>190.4427642822266</v>
+        <v>217.3411560058594</v>
       </c>
       <c r="B181" t="n">
-        <v>361.48</v>
+        <v>232.11</v>
       </c>
       <c r="C181" t="n">
-        <v>171.0372357177735</v>
+        <v>14.76884399414064</v>
       </c>
     </row>
     <row r="182">
       <c r="A182" t="n">
-        <v>178.2145538330078</v>
+        <v>276.5860595703125</v>
       </c>
       <c r="B182" t="n">
-        <v>361.48</v>
+        <v>250.57</v>
       </c>
       <c r="C182" t="n">
-        <v>183.2654461669922</v>
+        <v>26.01605957031251</v>
       </c>
     </row>
     <row r="183">
       <c r="A183" t="n">
-        <v>287.383056640625</v>
+        <v>290.1375427246094</v>
       </c>
       <c r="B183" t="n">
-        <v>279.11</v>
+        <v>275.62</v>
       </c>
       <c r="C183" t="n">
-        <v>8.273056640624986</v>
+        <v>14.51754272460937</v>
       </c>
     </row>
     <row r="184">
       <c r="A184" t="n">
-        <v>276.6048889160156</v>
+        <v>300.059814453125</v>
       </c>
       <c r="B184" t="n">
-        <v>265.66</v>
+        <v>294</v>
       </c>
       <c r="C184" t="n">
-        <v>10.9448889160156</v>
+        <v>6.059814453125</v>
       </c>
     </row>
     <row r="185">
       <c r="A185" t="n">
-        <v>261.30224609375</v>
+        <v>275.8364868164062</v>
       </c>
       <c r="B185" t="n">
-        <v>247.75</v>
+        <v>306.25</v>
       </c>
       <c r="C185" t="n">
-        <v>13.55224609375</v>
+        <v>30.41351318359375</v>
       </c>
     </row>
     <row r="186">
       <c r="A186" t="n">
-        <v>248.8310699462891</v>
+        <v>272.7057495117188</v>
       </c>
       <c r="B186" t="n">
-        <v>247.75</v>
+        <v>272.22</v>
       </c>
       <c r="C186" t="n">
-        <v>1.081069946289062</v>
+        <v>0.4857495117187227</v>
       </c>
     </row>
     <row r="187">
       <c r="A187" t="n">
-        <v>240.1075897216797</v>
+        <v>281.0840148925781</v>
       </c>
       <c r="B187" t="n">
-        <v>247.75</v>
+        <v>275.62</v>
       </c>
       <c r="C187" t="n">
-        <v>7.642410278320312</v>
+        <v>5.46401489257812</v>
       </c>
     </row>
     <row r="188">
       <c r="A188" t="n">
-        <v>233.3475952148438</v>
+        <v>289.3341674804688</v>
       </c>
       <c r="B188" t="n">
-        <v>242.31</v>
+        <v>279.11</v>
       </c>
       <c r="C188" t="n">
-        <v>8.962404785156252</v>
+        <v>10.22416748046874</v>
       </c>
     </row>
     <row r="189">
       <c r="A189" t="n">
-        <v>217.3411560058594</v>
+        <v>302.443359375</v>
       </c>
       <c r="B189" t="n">
-        <v>232.11</v>
+        <v>286.36</v>
       </c>
       <c r="C189" t="n">
-        <v>14.76884399414064</v>
+        <v>16.08335937499999</v>
       </c>
     </row>
     <row r="190">
       <c r="A190" t="n">
-        <v>206.5080261230469</v>
+        <v>321.4532165527344</v>
       </c>
       <c r="B190" t="n">
-        <v>204.17</v>
+        <v>297.97</v>
       </c>
       <c r="C190" t="n">
-        <v>2.338026123046888</v>
+        <v>23.48321655273435</v>
       </c>
     </row>
     <row r="191">
       <c r="A191" t="n">
-        <v>204.4027862548828</v>
+        <v>341.8348083496094</v>
       </c>
       <c r="B191" t="n">
-        <v>111.93</v>
+        <v>315</v>
       </c>
       <c r="C191" t="n">
-        <v>92.47278625488281</v>
+        <v>26.83480834960938</v>
       </c>
     </row>
     <row r="192">
       <c r="A192" t="n">
-        <v>268.1163635253906</v>
+        <v>356.6332092285156</v>
       </c>
       <c r="B192" t="n">
-        <v>111.93</v>
+        <v>339.23</v>
       </c>
       <c r="C192" t="n">
-        <v>156.1863635253906</v>
+        <v>17.40320922851561</v>
       </c>
     </row>
     <row r="193">
       <c r="A193" t="n">
-        <v>276.5860595703125</v>
+        <v>183.9189453125</v>
       </c>
       <c r="B193" t="n">
-        <v>204.17</v>
+        <v>350</v>
       </c>
       <c r="C193" t="n">
-        <v>72.41605957031251</v>
+        <v>166.0810546875</v>
       </c>
     </row>
     <row r="194">
       <c r="A194" t="n">
-        <v>290.1375427246094</v>
+        <v>187.4046936035156</v>
       </c>
       <c r="B194" t="n">
-        <v>275.62</v>
+        <v>367.5</v>
       </c>
       <c r="C194" t="n">
-        <v>14.51754272460937</v>
+        <v>180.0953063964844</v>
       </c>
     </row>
     <row r="195">
       <c r="A195" t="n">
-        <v>300.059814453125</v>
+        <v>0</v>
       </c>
       <c r="B195" t="n">
-        <v>275.62</v>
+        <v>380.17</v>
       </c>
       <c r="C195" t="n">
-        <v>24.439814453125</v>
-      </c>
-    </row>
-    <row r="196">
-      <c r="A196" t="n">
-        <v>275.8364868164062</v>
-      </c>
-      <c r="B196" t="n">
-        <v>275.62</v>
-      </c>
-      <c r="C196" t="n">
-        <v>0.2164868164062455</v>
-      </c>
-    </row>
-    <row r="197">
-      <c r="A197" t="n">
-        <v>295.107177734375</v>
-      </c>
-      <c r="B197" t="n">
-        <v>272.22</v>
-      </c>
-      <c r="C197" t="n">
-        <v>22.88717773437497</v>
-      </c>
-    </row>
-    <row r="198">
-      <c r="A198" t="n">
-        <v>276.9979858398438</v>
-      </c>
-      <c r="B198" t="n">
-        <v>272.22</v>
-      </c>
-      <c r="C198" t="n">
-        <v>4.777985839843723</v>
-      </c>
-    </row>
-    <row r="199">
-      <c r="A199" t="n">
-        <v>281.0840148925781</v>
-      </c>
-      <c r="B199" t="n">
-        <v>275.62</v>
-      </c>
-      <c r="C199" t="n">
-        <v>5.46401489257812</v>
-      </c>
-    </row>
-    <row r="200">
-      <c r="A200" t="n">
-        <v>289.3341674804688</v>
-      </c>
-      <c r="B200" t="n">
-        <v>279.11</v>
-      </c>
-      <c r="C200" t="n">
-        <v>10.22416748046874</v>
-      </c>
-    </row>
-    <row r="201">
-      <c r="A201" t="n">
-        <v>302.443359375</v>
-      </c>
-      <c r="B201" t="n">
-        <v>286.36</v>
-      </c>
-      <c r="C201" t="n">
-        <v>16.08335937499999</v>
-      </c>
-    </row>
-    <row r="202">
-      <c r="A202" t="n">
-        <v>321.4532165527344</v>
-      </c>
-      <c r="B202" t="n">
-        <v>297.97</v>
-      </c>
-      <c r="C202" t="n">
-        <v>23.48321655273435</v>
-      </c>
-    </row>
-    <row r="203">
-      <c r="A203" t="n">
-        <v>341.8348083496094</v>
-      </c>
-      <c r="B203" t="n">
-        <v>315</v>
-      </c>
-      <c r="C203" t="n">
-        <v>26.83480834960938</v>
-      </c>
-    </row>
-    <row r="204">
-      <c r="A204" t="n">
-        <v>356.6332092285156</v>
-      </c>
-      <c r="B204" t="n">
-        <v>339.23</v>
-      </c>
-      <c r="C204" t="n">
-        <v>17.40320922851561</v>
-      </c>
-    </row>
-    <row r="205">
-      <c r="A205" t="n">
-        <v>183.9189453125</v>
-      </c>
-      <c r="B205" t="n">
-        <v>350</v>
-      </c>
-      <c r="C205" t="n">
-        <v>166.0810546875</v>
-      </c>
-    </row>
-    <row r="206">
-      <c r="A206" t="n">
-        <v>187.4046936035156</v>
-      </c>
-      <c r="B206" t="n">
-        <v>350</v>
-      </c>
-      <c r="C206" t="n">
-        <v>162.5953063964844</v>
-      </c>
-    </row>
-    <row r="207">
-      <c r="A207" t="n">
-        <v>0</v>
-      </c>
-      <c r="B207" t="n">
-        <v>350</v>
-      </c>
-      <c r="C207" t="n">
-        <v>350</v>
+        <v>380.17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>